<commit_message>
avance recargoSaldo y solucion letra ñ
</commit_message>
<xml_diff>
--- a/Archivos Excel/archivo.xlsx
+++ b/Archivos Excel/archivo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sistemaInsuma\Pruebas\cargarExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E0C892-1A58-4AB6-8E0F-9A1A37B7B926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A96483-E248-4561-B670-EFAA46550A59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1890,6 +1892,27 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="45" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="46" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="44" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="43" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="32" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="33" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1933,27 +1956,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="4" borderId="33" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="45" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="46" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="44" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="43" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="32" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="33" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7831,7 +7833,7 @@
   </sheetPr>
   <dimension ref="A1:AM44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -7847,14 +7849,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="146" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
       <c r="AK1" s="7"/>
       <c r="AM1" s="6"/>
     </row>
@@ -7923,42 +7925,42 @@
       <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="140" t="s">
+      <c r="A6" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="142" t="s">
+      <c r="B6" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="155" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="144" t="s">
+      <c r="D6" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="146" t="s">
+      <c r="E6" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="150" t="s">
+      <c r="F6" s="157" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="155" t="s">
+      <c r="H6" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="157" t="s">
+      <c r="I6" s="142" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="141"/>
-      <c r="B7" s="143" t="s">
+      <c r="A7" s="148"/>
+      <c r="B7" s="150" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="149"/>
-      <c r="D7" s="145"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="151"/>
-      <c r="H7" s="156"/>
-      <c r="I7" s="158"/>
+      <c r="C7" s="156"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="154"/>
+      <c r="F7" s="158"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="143"/>
     </row>
     <row r="8" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
@@ -8932,13 +8934,13 @@
       <c r="I37" s="115"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="159" t="s">
+      <c r="A38" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="160"/>
-      <c r="C38" s="152"/>
-      <c r="D38" s="153"/>
-      <c r="E38" s="154"/>
+      <c r="B38" s="145"/>
+      <c r="C38" s="159"/>
+      <c r="D38" s="160"/>
+      <c r="E38" s="161"/>
       <c r="F38" s="35">
         <f>AVERAGE(F8:F35)</f>
         <v>4.4063588435374159</v>
@@ -8996,12 +8998,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
     <mergeCell ref="A40:F41"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -9010,6 +9006,12 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="C38:E38"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="F8:F37">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
recargoSaldo v1 y regPago v3
</commit_message>
<xml_diff>
--- a/Archivos Excel/archivo.xlsx
+++ b/Archivos Excel/archivo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sistemaInsuma\Pruebas\cargarExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A96483-E248-4561-B670-EFAA46550A59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2C574A-F72C-40D2-A538-626E98C28B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="102">
   <si>
     <t>No.</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t>ADRIAN CHAVEZ</t>
+  </si>
+  <si>
+    <t>BUÑUELOS ÑOÑO</t>
   </si>
 </sst>
 </file>
@@ -7833,8 +7836,8 @@
   </sheetPr>
   <dimension ref="A1:AM44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8590,9 +8593,8 @@
       <c r="A27" s="33">
         <v>20</v>
       </c>
-      <c r="B27" s="36" t="str">
-        <f>'PRIMER PARCIAL'!B28</f>
-        <v>RAMIREZ CISNEROS FERNANDO</v>
+      <c r="B27" s="36" t="s">
+        <v>101</v>
       </c>
       <c r="C27" s="77">
         <f>'PRIMER PARCIAL'!L28</f>

</xml_diff>